<commit_message>
Fix Data Driven Test by provided the expect
</commit_message>
<xml_diff>
--- a/test-data/OpenCart_DataTest.xlsx
+++ b/test-data/OpenCart_DataTest.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\JAVA\OpenCartV121\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C9F02B6-D0FF-4AB7-B2ED-5359047E191A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9364425-7972-47B9-9C15-934A00A284F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="10830" xr2:uid="{4E2415AC-3B95-4E0F-9366-9AADE586E554}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>username</t>
   </si>
@@ -42,15 +42,9 @@
     <t>Valid</t>
   </si>
   <si>
-    <t>fjhskjs</t>
-  </si>
-  <si>
     <t>Invalid</t>
   </si>
   <si>
-    <t>test1@gmail.com</t>
-  </si>
-  <si>
     <t>jhfdjhdj@gmail.com</t>
   </si>
   <si>
@@ -63,10 +57,13 @@
     <t>abc</t>
   </si>
   <si>
-    <t>test2@gmail.com</t>
-  </si>
-  <si>
-    <t>invalid</t>
+    <t>test1234@gmail.com</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>test23456@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -471,7 +468,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -500,15 +497,15 @@
         <v>1234</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>4</v>
@@ -516,24 +513,24 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -548,12 +545,8 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>